<commit_message>
ordinate cose ma ancora non funziona
</commit_message>
<xml_diff>
--- a/Source.xlsx
+++ b/Source.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/teo/Documents/GitHub/compilatore-piano-di-studi/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D7AE98E-0D6A-FA4E-B6BD-0BF9E86D49FE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96B0F733-B104-9F43-97B2-C0CC34446464}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="440" windowWidth="28800" windowHeight="16520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="103">
   <si>
     <t>Denominazione</t>
   </si>
@@ -317,9 +317,6 @@
   </si>
   <si>
     <t>COMPUTATIONAL TECHNIQUES FOR MOLECULAR MODELING</t>
-  </si>
-  <si>
-    <t>Gruppo_id</t>
   </si>
   <si>
     <t>REAL AND FUNCTIONAL ANALYSIS</t>
@@ -627,10 +624,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:G161"/>
+  <dimension ref="A1:F161"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" topLeftCell="A63" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="F86" sqref="F86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -638,7 +635,7 @@
     <col min="1" max="1" width="71.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -655,13 +652,10 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>11</v>
       </c>
@@ -677,12 +671,11 @@
       <c r="E2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="4">
-        <v>0</v>
-      </c>
-      <c r="G2" s="2"/>
-    </row>
-    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F2" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>11</v>
       </c>
@@ -699,11 +692,10 @@
         <v>61</v>
       </c>
       <c r="F3" s="4">
-        <v>3</v>
-      </c>
-      <c r="G3" s="4"/>
-    </row>
-    <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>54</v>
       </c>
@@ -719,12 +711,11 @@
       <c r="E4" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="F4" s="4">
-        <v>2</v>
-      </c>
-      <c r="G4" s="2"/>
-    </row>
-    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F4" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>54</v>
       </c>
@@ -743,9 +734,8 @@
       <c r="F5" s="4">
         <v>3</v>
       </c>
-      <c r="G5" s="4"/>
-    </row>
-    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>76</v>
       </c>
@@ -761,12 +751,9 @@
       <c r="E6" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="F6" s="4">
-        <v>3</v>
-      </c>
-      <c r="G6" s="4"/>
-    </row>
-    <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F6" s="4"/>
+    </row>
+    <row r="7" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>75</v>
       </c>
@@ -782,12 +769,9 @@
       <c r="E7" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="F7" s="4">
-        <v>3</v>
-      </c>
-      <c r="G7" s="4"/>
-    </row>
-    <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F7" s="4"/>
+    </row>
+    <row r="8" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>48</v>
       </c>
@@ -803,12 +787,11 @@
       <c r="E8" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="F8" s="4">
-        <v>2</v>
-      </c>
-      <c r="G8" s="2"/>
-    </row>
-    <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F8" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
         <v>48</v>
       </c>
@@ -825,11 +808,10 @@
         <v>61</v>
       </c>
       <c r="F9" s="4">
-        <v>3</v>
-      </c>
-      <c r="G9" s="4"/>
-    </row>
-    <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
         <v>85</v>
       </c>
@@ -846,11 +828,10 @@
         <v>61</v>
       </c>
       <c r="F10" s="4">
-        <v>3</v>
-      </c>
-      <c r="G10" s="4"/>
-    </row>
-    <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
         <v>95</v>
       </c>
@@ -866,14 +847,11 @@
       <c r="E11" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="F11" s="4">
-        <v>3</v>
-      </c>
-      <c r="G11" s="4"/>
-    </row>
-    <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F11" s="4"/>
+    </row>
+    <row r="12" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B12" s="4">
         <v>52496</v>
@@ -885,14 +863,11 @@
         <v>10</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="F12" s="4">
-        <v>5</v>
-      </c>
-      <c r="G12" s="4"/>
-    </row>
-    <row r="13" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>100</v>
+      </c>
+      <c r="F12" s="4"/>
+    </row>
+    <row r="13" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
         <v>93</v>
       </c>
@@ -908,12 +883,9 @@
       <c r="E13" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="F13" s="4">
-        <v>3</v>
-      </c>
-      <c r="G13" s="4"/>
-    </row>
-    <row r="14" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F13" s="4"/>
+    </row>
+    <row r="14" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
         <v>34</v>
       </c>
@@ -929,12 +901,9 @@
       <c r="E14" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="F14" s="4">
-        <v>1</v>
-      </c>
-      <c r="G14" s="4"/>
-    </row>
-    <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F14" s="4"/>
+    </row>
+    <row r="15" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
         <v>34</v>
       </c>
@@ -948,14 +917,11 @@
         <v>10</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="F15" s="4">
-        <v>5</v>
-      </c>
-      <c r="G15" s="4"/>
-    </row>
-    <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>100</v>
+      </c>
+      <c r="F15" s="4"/>
+    </row>
+    <row r="16" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
         <v>22</v>
       </c>
@@ -969,14 +935,11 @@
         <v>10</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="F16" s="4">
-        <v>5</v>
-      </c>
-      <c r="G16" s="4"/>
-    </row>
-    <row r="17" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>100</v>
+      </c>
+      <c r="F16" s="4"/>
+    </row>
+    <row r="17" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
         <v>22</v>
       </c>
@@ -992,12 +955,9 @@
       <c r="E17" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="F17" s="4">
-        <v>1</v>
-      </c>
-      <c r="G17" s="4"/>
-    </row>
-    <row r="18" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F17" s="4"/>
+    </row>
+    <row r="18" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
         <v>22</v>
       </c>
@@ -1013,12 +973,9 @@
       <c r="E18" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="F18" s="4">
-        <v>3</v>
-      </c>
-      <c r="G18" s="4"/>
-    </row>
-    <row r="19" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F18" s="4"/>
+    </row>
+    <row r="19" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
         <v>26</v>
       </c>
@@ -1034,14 +991,11 @@
       <c r="E19" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="F19" s="4">
-        <v>1</v>
-      </c>
-      <c r="G19" s="2">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F19" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
         <v>26</v>
       </c>
@@ -1058,13 +1012,10 @@
         <v>61</v>
       </c>
       <c r="F20" s="4">
-        <v>3</v>
-      </c>
-      <c r="G20" s="4">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
         <v>77</v>
       </c>
@@ -1081,11 +1032,10 @@
         <v>61</v>
       </c>
       <c r="F21" s="4">
-        <v>3</v>
-      </c>
-      <c r="G21" s="4"/>
-    </row>
-    <row r="22" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
         <v>40</v>
       </c>
@@ -1101,14 +1051,11 @@
       <c r="E22" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="F22" s="4">
-        <v>1</v>
-      </c>
-      <c r="G22" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+      <c r="F22" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="s">
         <v>40</v>
       </c>
@@ -1125,13 +1072,10 @@
         <v>61</v>
       </c>
       <c r="F23" s="4">
-        <v>3</v>
-      </c>
-      <c r="G23" s="4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A24" s="4" t="s">
         <v>42</v>
       </c>
@@ -1148,11 +1092,10 @@
         <v>61</v>
       </c>
       <c r="F24" s="4">
-        <v>3</v>
-      </c>
-      <c r="G24" s="4"/>
-    </row>
-    <row r="25" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A25" s="4" t="s">
         <v>13</v>
       </c>
@@ -1168,12 +1111,11 @@
       <c r="E25" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="F25" s="4">
-        <v>0</v>
-      </c>
-      <c r="G25" s="2"/>
-    </row>
-    <row r="26" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+      <c r="F25" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A26" s="4" t="s">
         <v>13</v>
       </c>
@@ -1189,12 +1131,11 @@
       <c r="E26" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="F26" s="4">
-        <v>2</v>
-      </c>
-      <c r="G26" s="2"/>
-    </row>
-    <row r="27" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+      <c r="F26" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A27" s="4" t="s">
         <v>13</v>
       </c>
@@ -1211,11 +1152,10 @@
         <v>61</v>
       </c>
       <c r="F27" s="4">
-        <v>3</v>
-      </c>
-      <c r="G27" s="4"/>
-    </row>
-    <row r="28" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A28" s="4" t="s">
         <v>80</v>
       </c>
@@ -1231,12 +1171,9 @@
       <c r="E28" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="F28" s="4">
-        <v>3</v>
-      </c>
-      <c r="G28" s="4"/>
-    </row>
-    <row r="29" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+      <c r="F28" s="4"/>
+    </row>
+    <row r="29" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A29" s="4" t="s">
         <v>94</v>
       </c>
@@ -1252,12 +1189,9 @@
       <c r="E29" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="F29" s="4">
-        <v>3</v>
-      </c>
-      <c r="G29" s="4"/>
-    </row>
-    <row r="30" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+      <c r="F29" s="4"/>
+    </row>
+    <row r="30" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A30" s="4" t="s">
         <v>34</v>
       </c>
@@ -1273,12 +1207,9 @@
       <c r="E30" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="F30" s="4">
-        <v>3</v>
-      </c>
-      <c r="G30" s="4"/>
-    </row>
-    <row r="31" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+      <c r="F30" s="4"/>
+    </row>
+    <row r="31" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A31" s="4" t="s">
         <v>80</v>
       </c>
@@ -1294,12 +1225,9 @@
       <c r="E31" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="F31" s="4">
-        <v>3</v>
-      </c>
-      <c r="G31" s="4"/>
-    </row>
-    <row r="32" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+      <c r="F31" s="4"/>
+    </row>
+    <row r="32" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A32" s="4" t="s">
         <v>94</v>
       </c>
@@ -1315,12 +1243,9 @@
       <c r="E32" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="F32" s="4">
-        <v>3</v>
-      </c>
-      <c r="G32" s="4"/>
-    </row>
-    <row r="33" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+      <c r="F32" s="4"/>
+    </row>
+    <row r="33" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A33" s="4" t="s">
         <v>73</v>
       </c>
@@ -1336,12 +1261,9 @@
       <c r="E33" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="F33" s="4">
-        <v>3</v>
-      </c>
-      <c r="G33" s="4"/>
-    </row>
-    <row r="34" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+      <c r="F33" s="4"/>
+    </row>
+    <row r="34" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A34" s="4" t="s">
         <v>51</v>
       </c>
@@ -1357,12 +1279,9 @@
       <c r="E34" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="F34" s="4">
-        <v>2</v>
-      </c>
-      <c r="G34" s="2"/>
-    </row>
-    <row r="35" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+      <c r="F34" s="2"/>
+    </row>
+    <row r="35" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A35" s="4" t="s">
         <v>51</v>
       </c>
@@ -1378,12 +1297,9 @@
       <c r="E35" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="F35" s="4">
-        <v>3</v>
-      </c>
-      <c r="G35" s="4"/>
-    </row>
-    <row r="36" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+      <c r="F35" s="4"/>
+    </row>
+    <row r="36" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A36" s="4" t="s">
         <v>19</v>
       </c>
@@ -1400,13 +1316,10 @@
         <v>20</v>
       </c>
       <c r="F36" s="4">
-        <v>4</v>
-      </c>
-      <c r="G36" s="4">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A37" s="4" t="s">
         <v>19</v>
       </c>
@@ -1422,14 +1335,11 @@
       <c r="E37" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="F37" s="4">
-        <v>1</v>
-      </c>
-      <c r="G37" s="2">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+      <c r="F37" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A38" s="4" t="s">
         <v>32</v>
       </c>
@@ -1445,12 +1355,9 @@
       <c r="E38" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="F38" s="4">
-        <v>1</v>
-      </c>
-      <c r="G38" s="4"/>
-    </row>
-    <row r="39" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+      <c r="F38" s="4"/>
+    </row>
+    <row r="39" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A39" s="4" t="s">
         <v>32</v>
       </c>
@@ -1466,12 +1373,9 @@
       <c r="E39" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="F39" s="4">
-        <v>3</v>
-      </c>
-      <c r="G39" s="4"/>
-    </row>
-    <row r="40" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+      <c r="F39" s="4"/>
+    </row>
+    <row r="40" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A40" s="4" t="s">
         <v>32</v>
       </c>
@@ -1485,14 +1389,11 @@
         <v>8</v>
       </c>
       <c r="E40" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="F40" s="4">
-        <v>5</v>
-      </c>
-      <c r="G40" s="4"/>
-    </row>
-    <row r="41" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+        <v>100</v>
+      </c>
+      <c r="F40" s="4"/>
+    </row>
+    <row r="41" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A41" s="4" t="s">
         <v>57</v>
       </c>
@@ -1508,12 +1409,9 @@
       <c r="E41" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="F41" s="4">
-        <v>2</v>
-      </c>
-      <c r="G41" s="4"/>
-    </row>
-    <row r="42" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+      <c r="F41" s="4"/>
+    </row>
+    <row r="42" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A42" s="4" t="s">
         <v>57</v>
       </c>
@@ -1529,12 +1427,9 @@
       <c r="E42" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="F42" s="4">
-        <v>3</v>
-      </c>
-      <c r="G42" s="4"/>
-    </row>
-    <row r="43" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+      <c r="F42" s="4"/>
+    </row>
+    <row r="43" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A43" s="4" t="s">
         <v>18</v>
       </c>
@@ -1550,12 +1445,9 @@
       <c r="E43" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="F43" s="4">
-        <v>0</v>
-      </c>
-      <c r="G43" s="2"/>
-    </row>
-    <row r="44" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+      <c r="F43" s="2"/>
+    </row>
+    <row r="44" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A44" s="4" t="s">
         <v>18</v>
       </c>
@@ -1571,12 +1463,9 @@
       <c r="E44" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="F44" s="4">
-        <v>3</v>
-      </c>
-      <c r="G44" s="4"/>
-    </row>
-    <row r="45" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+      <c r="F44" s="4"/>
+    </row>
+    <row r="45" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A45" s="4" t="s">
         <v>8</v>
       </c>
@@ -1592,14 +1481,11 @@
       <c r="E45" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="F45" s="4">
-        <v>0</v>
-      </c>
-      <c r="G45" s="2">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+      <c r="F45" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A46" s="4" t="s">
         <v>8</v>
       </c>
@@ -1615,14 +1501,11 @@
       <c r="E46" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="F46" s="4">
-        <v>2</v>
-      </c>
-      <c r="G46" s="2">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+      <c r="F46" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A47" s="4" t="s">
         <v>8</v>
       </c>
@@ -1639,13 +1522,10 @@
         <v>61</v>
       </c>
       <c r="F47" s="4">
-        <v>3</v>
-      </c>
-      <c r="G47" s="4">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A48" s="4" t="s">
         <v>90</v>
       </c>
@@ -1661,12 +1541,9 @@
       <c r="E48" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="F48" s="4">
-        <v>3</v>
-      </c>
-      <c r="G48" s="4"/>
-    </row>
-    <row r="49" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+      <c r="F48" s="4"/>
+    </row>
+    <row r="49" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A49" s="4" t="s">
         <v>92</v>
       </c>
@@ -1682,12 +1559,9 @@
       <c r="E49" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="F49" s="4">
-        <v>3</v>
-      </c>
-      <c r="G49" s="4"/>
-    </row>
-    <row r="50" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+      <c r="F49" s="4"/>
+    </row>
+    <row r="50" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A50" s="4" t="s">
         <v>19</v>
       </c>
@@ -1704,13 +1578,10 @@
         <v>61</v>
       </c>
       <c r="F50" s="4">
-        <v>3</v>
-      </c>
-      <c r="G50" s="4">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A51" s="4" t="s">
         <v>89</v>
       </c>
@@ -1726,12 +1597,9 @@
       <c r="E51" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="F51" s="4">
-        <v>3</v>
-      </c>
-      <c r="G51" s="4"/>
-    </row>
-    <row r="52" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+      <c r="F51" s="4"/>
+    </row>
+    <row r="52" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A52" s="4" t="s">
         <v>41</v>
       </c>
@@ -1747,14 +1615,11 @@
       <c r="E52" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="F52" s="4">
-        <v>1</v>
-      </c>
-      <c r="G52" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+      <c r="F52" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A53" s="4" t="s">
         <v>41</v>
       </c>
@@ -1771,13 +1636,10 @@
         <v>61</v>
       </c>
       <c r="F53" s="4">
-        <v>3</v>
-      </c>
-      <c r="G53" s="4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A54" s="4" t="s">
         <v>69</v>
       </c>
@@ -1793,12 +1655,9 @@
       <c r="E54" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="F54" s="4">
-        <v>3</v>
-      </c>
-      <c r="G54" s="4"/>
-    </row>
-    <row r="55" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+      <c r="F54" s="4"/>
+    </row>
+    <row r="55" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A55" s="4" t="s">
         <v>52</v>
       </c>
@@ -1814,12 +1673,9 @@
       <c r="E55" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="F55" s="4">
-        <v>2</v>
-      </c>
-      <c r="G55" s="2"/>
-    </row>
-    <row r="56" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+      <c r="F55" s="2"/>
+    </row>
+    <row r="56" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A56" s="4" t="s">
         <v>52</v>
       </c>
@@ -1835,12 +1691,9 @@
       <c r="E56" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="F56" s="4">
-        <v>3</v>
-      </c>
-      <c r="G56" s="4"/>
-    </row>
-    <row r="57" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+      <c r="F56" s="4"/>
+    </row>
+    <row r="57" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A57" s="4" t="s">
         <v>30</v>
       </c>
@@ -1856,14 +1709,11 @@
       <c r="E57" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="F57" s="4">
-        <v>1</v>
-      </c>
-      <c r="G57" s="2">
+      <c r="F57" s="2">
         <v>4</v>
       </c>
     </row>
-    <row r="58" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A58" s="4" t="s">
         <v>30</v>
       </c>
@@ -1880,13 +1730,10 @@
         <v>61</v>
       </c>
       <c r="F58" s="4">
-        <v>3</v>
-      </c>
-      <c r="G58" s="4">
         <v>4</v>
       </c>
     </row>
-    <row r="59" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A59" s="4" t="s">
         <v>30</v>
       </c>
@@ -1902,14 +1749,11 @@
       <c r="E59" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="F59" s="4">
-        <v>1</v>
-      </c>
-      <c r="G59" s="2">
+      <c r="F59" s="2">
         <v>4</v>
       </c>
     </row>
-    <row r="60" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A60" s="4" t="s">
         <v>30</v>
       </c>
@@ -1926,13 +1770,10 @@
         <v>61</v>
       </c>
       <c r="F60" s="4">
-        <v>3</v>
-      </c>
-      <c r="G60" s="4">
         <v>4</v>
       </c>
     </row>
-    <row r="61" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A61" s="4" t="s">
         <v>9</v>
       </c>
@@ -1948,14 +1789,11 @@
       <c r="E61" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="F61" s="4">
-        <v>1</v>
-      </c>
-      <c r="G61" s="2">
+      <c r="F61" s="2">
         <v>3</v>
       </c>
     </row>
-    <row r="62" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A62" s="4" t="s">
         <v>9</v>
       </c>
@@ -1974,11 +1812,8 @@
       <c r="F62" s="4">
         <v>3</v>
       </c>
-      <c r="G62" s="4">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="63" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+    </row>
+    <row r="63" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A63" s="4" t="s">
         <v>9</v>
       </c>
@@ -1994,14 +1829,11 @@
       <c r="E63" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="F63" s="4">
-        <v>0</v>
-      </c>
-      <c r="G63" s="2">
+      <c r="F63" s="2">
         <v>4</v>
       </c>
     </row>
-    <row r="64" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A64" s="4" t="s">
         <v>14</v>
       </c>
@@ -2017,14 +1849,11 @@
       <c r="E64" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="F64" s="4">
-        <v>1</v>
-      </c>
-      <c r="G64" s="2">
+      <c r="F64" s="2">
         <v>4</v>
       </c>
     </row>
-    <row r="65" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A65" s="4" t="s">
         <v>14</v>
       </c>
@@ -2041,13 +1870,10 @@
         <v>61</v>
       </c>
       <c r="F65" s="4">
-        <v>3</v>
-      </c>
-      <c r="G65" s="4">
         <v>4</v>
       </c>
     </row>
-    <row r="66" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A66" s="4" t="s">
         <v>14</v>
       </c>
@@ -2063,14 +1889,11 @@
       <c r="E66" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="F66" s="4">
-        <v>0</v>
-      </c>
-      <c r="G66" s="2">
+      <c r="F66" s="2">
         <v>4</v>
       </c>
     </row>
-    <row r="67" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A67" s="4" t="s">
         <v>39</v>
       </c>
@@ -2086,12 +1909,9 @@
       <c r="E67" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="F67" s="4">
-        <v>1</v>
-      </c>
-      <c r="G67" s="2"/>
-    </row>
-    <row r="68" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+      <c r="F67" s="2"/>
+    </row>
+    <row r="68" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A68" s="4" t="s">
         <v>98</v>
       </c>
@@ -2107,12 +1927,9 @@
       <c r="E68" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="F68" s="4">
-        <v>3</v>
-      </c>
-      <c r="G68" s="4"/>
-    </row>
-    <row r="69" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+      <c r="F68" s="4"/>
+    </row>
+    <row r="69" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A69" s="4" t="s">
         <v>38</v>
       </c>
@@ -2128,12 +1945,9 @@
       <c r="E69" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="F69" s="4">
-        <v>1</v>
-      </c>
-      <c r="G69" s="2"/>
-    </row>
-    <row r="70" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+      <c r="F69" s="2"/>
+    </row>
+    <row r="70" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A70" s="4" t="s">
         <v>47</v>
       </c>
@@ -2149,12 +1963,9 @@
       <c r="E70" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="F70" s="4">
-        <v>2</v>
-      </c>
-      <c r="G70" s="2"/>
-    </row>
-    <row r="71" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+      <c r="F70" s="2"/>
+    </row>
+    <row r="71" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A71" s="4" t="s">
         <v>47</v>
       </c>
@@ -2170,12 +1981,9 @@
       <c r="E71" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="F71" s="4">
-        <v>3</v>
-      </c>
-      <c r="G71" s="4"/>
-    </row>
-    <row r="72" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+      <c r="F71" s="4"/>
+    </row>
+    <row r="72" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A72" s="4" t="s">
         <v>42</v>
       </c>
@@ -2191,14 +1999,11 @@
       <c r="E72" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="F72" s="4">
-        <v>1</v>
-      </c>
-      <c r="G72" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="73" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+      <c r="F72" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A73" s="4" t="s">
         <v>42</v>
       </c>
@@ -2215,13 +2020,10 @@
         <v>61</v>
       </c>
       <c r="F73" s="4">
-        <v>3</v>
-      </c>
-      <c r="G73" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="74" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A74" s="4" t="s">
         <v>83</v>
       </c>
@@ -2238,11 +2040,10 @@
         <v>61</v>
       </c>
       <c r="F74" s="4">
-        <v>3</v>
-      </c>
-      <c r="G74" s="4"/>
-    </row>
-    <row r="75" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A75" s="4" t="s">
         <v>84</v>
       </c>
@@ -2259,11 +2060,10 @@
         <v>61</v>
       </c>
       <c r="F75" s="4">
-        <v>3</v>
-      </c>
-      <c r="G75" s="4"/>
-    </row>
-    <row r="76" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A76" s="4" t="s">
         <v>84</v>
       </c>
@@ -2280,11 +2080,10 @@
         <v>61</v>
       </c>
       <c r="F76" s="4">
-        <v>3</v>
-      </c>
-      <c r="G76" s="4"/>
-    </row>
-    <row r="77" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A77" s="4" t="s">
         <v>83</v>
       </c>
@@ -2301,11 +2100,10 @@
         <v>61</v>
       </c>
       <c r="F77" s="4">
-        <v>3</v>
-      </c>
-      <c r="G77" s="4"/>
-    </row>
-    <row r="78" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A78" s="4" t="s">
         <v>73</v>
       </c>
@@ -2322,11 +2120,10 @@
         <v>61</v>
       </c>
       <c r="F78" s="4">
-        <v>3</v>
-      </c>
-      <c r="G78" s="4"/>
-    </row>
-    <row r="79" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A79" s="4" t="s">
         <v>66</v>
       </c>
@@ -2343,11 +2140,10 @@
         <v>61</v>
       </c>
       <c r="F79" s="4">
-        <v>3</v>
-      </c>
-      <c r="G79" s="4"/>
-    </row>
-    <row r="80" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A80" s="4" t="s">
         <v>62</v>
       </c>
@@ -2364,13 +2160,10 @@
         <v>61</v>
       </c>
       <c r="F80" s="4">
-        <v>3</v>
-      </c>
-      <c r="G80" s="4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="81" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A81" s="4" t="s">
         <v>46</v>
       </c>
@@ -2386,12 +2179,11 @@
       <c r="E81" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="F81" s="4">
-        <v>2</v>
-      </c>
-      <c r="G81" s="2"/>
-    </row>
-    <row r="82" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+      <c r="F81" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A82" s="4" t="s">
         <v>46</v>
       </c>
@@ -2408,11 +2200,10 @@
         <v>61</v>
       </c>
       <c r="F82" s="4">
-        <v>3</v>
-      </c>
-      <c r="G82" s="4"/>
-    </row>
-    <row r="83" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A83" s="4" t="s">
         <v>79</v>
       </c>
@@ -2429,11 +2220,10 @@
         <v>61</v>
       </c>
       <c r="F83" s="4">
-        <v>3</v>
-      </c>
-      <c r="G83" s="4"/>
-    </row>
-    <row r="84" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A84" s="4" t="s">
         <v>79</v>
       </c>
@@ -2450,11 +2240,10 @@
         <v>61</v>
       </c>
       <c r="F84" s="4">
-        <v>3</v>
-      </c>
-      <c r="G84" s="4"/>
-    </row>
-    <row r="85" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A85" s="4" t="s">
         <v>97</v>
       </c>
@@ -2471,11 +2260,10 @@
         <v>61</v>
       </c>
       <c r="F85" s="4">
-        <v>3</v>
-      </c>
-      <c r="G85" s="4"/>
-    </row>
-    <row r="86" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A86" s="4" t="s">
         <v>10</v>
       </c>
@@ -2491,14 +2279,11 @@
       <c r="E86" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="F86" s="4">
-        <v>0</v>
-      </c>
-      <c r="G86" s="2">
+      <c r="F86" s="2">
         <v>3</v>
       </c>
     </row>
-    <row r="87" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A87" s="4" t="s">
         <v>10</v>
       </c>
@@ -2514,14 +2299,11 @@
       <c r="E87" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="F87" s="4">
-        <v>2</v>
-      </c>
-      <c r="G87" s="2">
+      <c r="F87" s="2">
         <v>3</v>
       </c>
     </row>
-    <row r="88" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A88" s="4" t="s">
         <v>10</v>
       </c>
@@ -2540,11 +2322,8 @@
       <c r="F88" s="4">
         <v>3</v>
       </c>
-      <c r="G88" s="4">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="89" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+    </row>
+    <row r="89" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A89" s="4" t="s">
         <v>59</v>
       </c>
@@ -2560,14 +2339,11 @@
       <c r="E89" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="F89" s="4">
-        <v>2</v>
-      </c>
-      <c r="G89" s="2">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="90" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+      <c r="F89" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A90" s="4" t="s">
         <v>59</v>
       </c>
@@ -2584,13 +2360,10 @@
         <v>61</v>
       </c>
       <c r="F90" s="4">
-        <v>3</v>
-      </c>
-      <c r="G90" s="4">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="91" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A91" s="4" t="s">
         <v>15</v>
       </c>
@@ -2606,14 +2379,11 @@
       <c r="E91" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="F91" s="4">
-        <v>0</v>
-      </c>
-      <c r="G91" s="2">
+      <c r="F91" s="2">
         <v>3</v>
       </c>
     </row>
-    <row r="92" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A92" s="4" t="s">
         <v>15</v>
       </c>
@@ -2629,14 +2399,11 @@
       <c r="E92" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="F92" s="4">
-        <v>2</v>
-      </c>
-      <c r="G92" s="2">
+      <c r="F92" s="2">
         <v>3</v>
       </c>
     </row>
-    <row r="93" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A93" s="4" t="s">
         <v>15</v>
       </c>
@@ -2655,11 +2422,8 @@
       <c r="F93" s="4">
         <v>3</v>
       </c>
-      <c r="G93" s="4">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="94" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+    </row>
+    <row r="94" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A94" s="4" t="s">
         <v>91</v>
       </c>
@@ -2675,12 +2439,9 @@
       <c r="E94" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="F94" s="4">
-        <v>3</v>
-      </c>
-      <c r="G94" s="4"/>
-    </row>
-    <row r="95" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+      <c r="F94" s="4"/>
+    </row>
+    <row r="95" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A95" s="4" t="s">
         <v>96</v>
       </c>
@@ -2696,12 +2457,9 @@
       <c r="E95" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="F95" s="4">
-        <v>3</v>
-      </c>
-      <c r="G95" s="4"/>
-    </row>
-    <row r="96" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+      <c r="F95" s="4"/>
+    </row>
+    <row r="96" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A96" s="4" t="s">
         <v>6</v>
       </c>
@@ -2717,12 +2475,9 @@
       <c r="E96" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="F96" s="4">
-        <v>0</v>
-      </c>
-      <c r="G96" s="2"/>
-    </row>
-    <row r="97" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+      <c r="F96" s="2"/>
+    </row>
+    <row r="97" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A97" s="4" t="s">
         <v>78</v>
       </c>
@@ -2739,13 +2494,10 @@
         <v>61</v>
       </c>
       <c r="F97" s="4">
-        <v>3</v>
-      </c>
-      <c r="G97" s="4">
         <v>4</v>
       </c>
     </row>
-    <row r="98" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A98" s="4" t="s">
         <v>50</v>
       </c>
@@ -2761,12 +2513,9 @@
       <c r="E98" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="F98" s="4">
-        <v>2</v>
-      </c>
-      <c r="G98" s="2"/>
-    </row>
-    <row r="99" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+      <c r="F98" s="2"/>
+    </row>
+    <row r="99" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A99" s="4" t="s">
         <v>50</v>
       </c>
@@ -2782,12 +2531,9 @@
       <c r="E99" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="F99" s="4">
-        <v>3</v>
-      </c>
-      <c r="G99" s="4"/>
-    </row>
-    <row r="100" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+      <c r="F99" s="4"/>
+    </row>
+    <row r="100" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A100" s="4" t="s">
         <v>44</v>
       </c>
@@ -2803,12 +2549,9 @@
       <c r="E100" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="F100" s="4">
-        <v>1</v>
-      </c>
-      <c r="G100" s="2"/>
-    </row>
-    <row r="101" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+      <c r="F100" s="2"/>
+    </row>
+    <row r="101" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A101" s="4" t="s">
         <v>44</v>
       </c>
@@ -2824,12 +2567,9 @@
       <c r="E101" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="F101" s="4">
-        <v>3</v>
-      </c>
-      <c r="G101" s="4"/>
-    </row>
-    <row r="102" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+      <c r="F101" s="4"/>
+    </row>
+    <row r="102" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A102" s="4" t="s">
         <v>49</v>
       </c>
@@ -2845,12 +2585,9 @@
       <c r="E102" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="F102" s="4">
-        <v>2</v>
-      </c>
-      <c r="G102" s="2"/>
-    </row>
-    <row r="103" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+      <c r="F102" s="2"/>
+    </row>
+    <row r="103" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A103" s="4" t="s">
         <v>49</v>
       </c>
@@ -2866,12 +2603,9 @@
       <c r="E103" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="F103" s="4">
-        <v>3</v>
-      </c>
-      <c r="G103" s="4"/>
-    </row>
-    <row r="104" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+      <c r="F103" s="4"/>
+    </row>
+    <row r="104" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A104" s="4" t="s">
         <v>86</v>
       </c>
@@ -2887,12 +2621,9 @@
       <c r="E104" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="F104" s="4">
-        <v>3</v>
-      </c>
-      <c r="G104" s="4"/>
-    </row>
-    <row r="105" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+      <c r="F104" s="4"/>
+    </row>
+    <row r="105" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A105" s="4" t="s">
         <v>56</v>
       </c>
@@ -2908,14 +2639,11 @@
       <c r="E105" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="F105" s="4">
-        <v>2</v>
-      </c>
-      <c r="G105" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="106" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+      <c r="F105" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A106" s="4" t="s">
         <v>56</v>
       </c>
@@ -2932,13 +2660,10 @@
         <v>61</v>
       </c>
       <c r="F106" s="4">
-        <v>3</v>
-      </c>
-      <c r="G106" s="4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="107" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A107" s="4" t="s">
         <v>16</v>
       </c>
@@ -2954,14 +2679,11 @@
       <c r="E107" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="F107" s="4">
-        <v>0</v>
-      </c>
-      <c r="G107" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="108" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+      <c r="F107" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A108" s="4" t="s">
         <v>16</v>
       </c>
@@ -2980,11 +2702,8 @@
       <c r="F108" s="4">
         <v>2</v>
       </c>
-      <c r="G108" s="4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="109" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+    </row>
+    <row r="109" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A109" s="4" t="s">
         <v>16</v>
       </c>
@@ -3001,13 +2720,10 @@
         <v>61</v>
       </c>
       <c r="F109" s="4">
-        <v>3</v>
-      </c>
-      <c r="G109" s="4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="110" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A110" s="4" t="s">
         <v>87</v>
       </c>
@@ -3023,12 +2739,9 @@
       <c r="E110" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="F110" s="4">
-        <v>3</v>
-      </c>
-      <c r="G110" s="4"/>
-    </row>
-    <row r="111" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+      <c r="F110" s="4"/>
+    </row>
+    <row r="111" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A111" s="4" t="s">
         <v>60</v>
       </c>
@@ -3044,12 +2757,9 @@
       <c r="E111" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="F111" s="4">
-        <v>3</v>
-      </c>
-      <c r="G111" s="4"/>
-    </row>
-    <row r="112" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+      <c r="F111" s="4"/>
+    </row>
+    <row r="112" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A112" s="4" t="s">
         <v>27</v>
       </c>
@@ -3065,12 +2775,9 @@
       <c r="E112" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="F112" s="4">
-        <v>1</v>
-      </c>
-      <c r="G112" s="2"/>
-    </row>
-    <row r="113" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+      <c r="F112" s="2"/>
+    </row>
+    <row r="113" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A113" s="4" t="s">
         <v>27</v>
       </c>
@@ -3086,12 +2793,9 @@
       <c r="E113" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="F113" s="4">
-        <v>3</v>
-      </c>
-      <c r="G113" s="4"/>
-    </row>
-    <row r="114" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+      <c r="F113" s="4"/>
+    </row>
+    <row r="114" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A114" s="4" t="s">
         <v>12</v>
       </c>
@@ -3107,12 +2811,9 @@
       <c r="E114" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="F114" s="4">
-        <v>0</v>
-      </c>
-      <c r="G114" s="2"/>
-    </row>
-    <row r="115" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+      <c r="F114" s="2"/>
+    </row>
+    <row r="115" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A115" s="4" t="s">
         <v>12</v>
       </c>
@@ -3128,12 +2829,9 @@
       <c r="E115" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="F115" s="4">
-        <v>3</v>
-      </c>
-      <c r="G115" s="4"/>
-    </row>
-    <row r="116" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+      <c r="F115" s="4"/>
+    </row>
+    <row r="116" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A116" s="4" t="s">
         <v>25</v>
       </c>
@@ -3149,14 +2847,11 @@
       <c r="E116" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="F116" s="4">
-        <v>1</v>
-      </c>
-      <c r="G116" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="117" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+      <c r="F116" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="117" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A117" s="4" t="s">
         <v>25</v>
       </c>
@@ -3173,13 +2868,10 @@
         <v>61</v>
       </c>
       <c r="F117" s="4">
-        <v>3</v>
-      </c>
-      <c r="G117" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="118" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="118" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A118" s="4" t="s">
         <v>70</v>
       </c>
@@ -3195,12 +2887,9 @@
       <c r="E118" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="F118" s="4">
-        <v>3</v>
-      </c>
-      <c r="G118" s="4"/>
-    </row>
-    <row r="119" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+      <c r="F118" s="4"/>
+    </row>
+    <row r="119" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A119" s="4" t="s">
         <v>68</v>
       </c>
@@ -3216,14 +2905,11 @@
       <c r="E119" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="F119" s="4">
-        <v>3</v>
-      </c>
-      <c r="G119" s="4"/>
-    </row>
-    <row r="120" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+      <c r="F119" s="4"/>
+    </row>
+    <row r="120" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A120" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B120" s="4">
         <v>95958</v>
@@ -3235,14 +2921,11 @@
         <v>8</v>
       </c>
       <c r="E120" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="F120" s="5">
-        <v>5</v>
-      </c>
-      <c r="G120" s="4"/>
-    </row>
-    <row r="121" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+        <v>100</v>
+      </c>
+      <c r="F120" s="4"/>
+    </row>
+    <row r="121" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A121" s="4" t="s">
         <v>33</v>
       </c>
@@ -3258,12 +2941,9 @@
       <c r="E121" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="F121" s="4">
-        <v>1</v>
-      </c>
-      <c r="G121" s="2"/>
-    </row>
-    <row r="122" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+      <c r="F121" s="2"/>
+    </row>
+    <row r="122" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A122" s="4" t="s">
         <v>33</v>
       </c>
@@ -3279,12 +2959,9 @@
       <c r="E122" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="F122" s="4">
-        <v>3</v>
-      </c>
-      <c r="G122" s="4"/>
-    </row>
-    <row r="123" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+      <c r="F122" s="4"/>
+    </row>
+    <row r="123" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A123" s="4" t="s">
         <v>43</v>
       </c>
@@ -3300,14 +2977,11 @@
       <c r="E123" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="F123" s="4">
-        <v>1</v>
-      </c>
-      <c r="G123" s="2">
+      <c r="F123" s="2">
         <v>4</v>
       </c>
     </row>
-    <row r="124" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A124" s="4" t="s">
         <v>43</v>
       </c>
@@ -3324,13 +2998,10 @@
         <v>61</v>
       </c>
       <c r="F124" s="4">
-        <v>3</v>
-      </c>
-      <c r="G124" s="4">
         <v>4</v>
       </c>
     </row>
-    <row r="125" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A125" s="4" t="s">
         <v>31</v>
       </c>
@@ -3346,14 +3017,11 @@
       <c r="E125" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="F125" s="4">
-        <v>1</v>
-      </c>
-      <c r="G125" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="126" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+      <c r="F125" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="126" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A126" s="4" t="s">
         <v>31</v>
       </c>
@@ -3369,12 +3037,9 @@
       <c r="E126" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="F126" s="4">
-        <v>3</v>
-      </c>
-      <c r="G126" s="4"/>
-    </row>
-    <row r="127" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+      <c r="F126" s="4"/>
+    </row>
+    <row r="127" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A127" s="4" t="s">
         <v>63</v>
       </c>
@@ -3390,12 +3055,9 @@
       <c r="E127" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="F127" s="4">
-        <v>3</v>
-      </c>
-      <c r="G127" s="4"/>
-    </row>
-    <row r="128" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+      <c r="F127" s="4"/>
+    </row>
+    <row r="128" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A128" s="4" t="s">
         <v>28</v>
       </c>
@@ -3412,13 +3074,10 @@
         <v>61</v>
       </c>
       <c r="F128" s="4">
-        <v>3</v>
-      </c>
-      <c r="G128" s="4">
         <v>4</v>
       </c>
     </row>
-    <row r="129" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A129" s="4" t="s">
         <v>28</v>
       </c>
@@ -3434,14 +3093,11 @@
       <c r="E129" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="F129" s="4">
-        <v>1</v>
-      </c>
-      <c r="G129" s="2">
+      <c r="F129" s="2">
         <v>4</v>
       </c>
     </row>
-    <row r="130" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A130" s="4" t="s">
         <v>64</v>
       </c>
@@ -3457,12 +3113,9 @@
       <c r="E130" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="F130" s="4">
-        <v>3</v>
-      </c>
-      <c r="G130" s="4"/>
-    </row>
-    <row r="131" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+      <c r="F130" s="4"/>
+    </row>
+    <row r="131" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A131" s="4" t="s">
         <v>65</v>
       </c>
@@ -3478,12 +3131,9 @@
       <c r="E131" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="F131" s="4">
-        <v>3</v>
-      </c>
-      <c r="G131" s="4"/>
-    </row>
-    <row r="132" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+      <c r="F131" s="4"/>
+    </row>
+    <row r="132" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A132" s="4" t="s">
         <v>58</v>
       </c>
@@ -3502,9 +3152,8 @@
       <c r="F132" s="4">
         <v>2</v>
       </c>
-      <c r="G132" s="4"/>
-    </row>
-    <row r="133" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+    </row>
+    <row r="133" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A133" s="4" t="s">
         <v>58</v>
       </c>
@@ -3521,11 +3170,10 @@
         <v>61</v>
       </c>
       <c r="F133" s="4">
-        <v>3</v>
-      </c>
-      <c r="G133" s="4"/>
-    </row>
-    <row r="134" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="134" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A134" s="4" t="s">
         <v>58</v>
       </c>
@@ -3539,14 +3187,13 @@
         <v>10</v>
       </c>
       <c r="E134" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F134" s="4">
-        <v>5</v>
-      </c>
-      <c r="G134" s="4"/>
-    </row>
-    <row r="135" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="135" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A135" s="4" t="s">
         <v>37</v>
       </c>
@@ -3562,12 +3209,11 @@
       <c r="E135" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="F135" s="4">
-        <v>1</v>
-      </c>
-      <c r="G135" s="2"/>
-    </row>
-    <row r="136" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+      <c r="F135" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="136" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A136" s="4" t="s">
         <v>37</v>
       </c>
@@ -3584,11 +3230,10 @@
         <v>61</v>
       </c>
       <c r="F136" s="4">
-        <v>3</v>
-      </c>
-      <c r="G136" s="4"/>
-    </row>
-    <row r="137" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="137" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A137" s="4" t="s">
         <v>82</v>
       </c>
@@ -3605,11 +3250,10 @@
         <v>61</v>
       </c>
       <c r="F137" s="4">
-        <v>3</v>
-      </c>
-      <c r="G137" s="4"/>
-    </row>
-    <row r="138" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="138" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A138" s="4" t="s">
         <v>53</v>
       </c>
@@ -3625,12 +3269,11 @@
       <c r="E138" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="F138" s="4">
-        <v>2</v>
-      </c>
-      <c r="G138" s="2"/>
-    </row>
-    <row r="139" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+      <c r="F138" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="139" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A139" s="4" t="s">
         <v>53</v>
       </c>
@@ -3647,11 +3290,10 @@
         <v>61</v>
       </c>
       <c r="F139" s="4">
-        <v>3</v>
-      </c>
-      <c r="G139" s="4"/>
-    </row>
-    <row r="140" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="140" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A140" s="4" t="s">
         <v>67</v>
       </c>
@@ -3668,11 +3310,10 @@
         <v>61</v>
       </c>
       <c r="F140" s="4">
-        <v>3</v>
-      </c>
-      <c r="G140" s="4"/>
-    </row>
-    <row r="141" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="141" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A141" s="4" t="s">
         <v>72</v>
       </c>
@@ -3689,11 +3330,10 @@
         <v>61</v>
       </c>
       <c r="F141" s="4">
-        <v>3</v>
-      </c>
-      <c r="G141" s="4"/>
-    </row>
-    <row r="142" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="142" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A142" s="4" t="s">
         <v>55</v>
       </c>
@@ -3709,12 +3349,9 @@
       <c r="E142" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="F142" s="4">
-        <v>2</v>
-      </c>
-      <c r="G142" s="2"/>
-    </row>
-    <row r="143" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+      <c r="F142" s="2"/>
+    </row>
+    <row r="143" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A143" s="4" t="s">
         <v>55</v>
       </c>
@@ -3730,12 +3367,9 @@
       <c r="E143" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="F143" s="4">
-        <v>3</v>
-      </c>
-      <c r="G143" s="4"/>
-    </row>
-    <row r="144" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+      <c r="F143" s="4"/>
+    </row>
+    <row r="144" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A144" s="4" t="s">
         <v>29</v>
       </c>
@@ -3751,12 +3385,9 @@
       <c r="E144" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="F144" s="4">
-        <v>1</v>
-      </c>
-      <c r="G144" s="2"/>
-    </row>
-    <row r="145" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+      <c r="F144" s="2"/>
+    </row>
+    <row r="145" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A145" s="4" t="s">
         <v>29</v>
       </c>
@@ -3772,12 +3403,9 @@
       <c r="E145" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="F145" s="4">
-        <v>3</v>
-      </c>
-      <c r="G145" s="4"/>
-    </row>
-    <row r="146" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+      <c r="F145" s="4"/>
+    </row>
+    <row r="146" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A146" s="4" t="s">
         <v>35</v>
       </c>
@@ -3793,12 +3421,9 @@
       <c r="E146" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="F146" s="4">
-        <v>1</v>
-      </c>
-      <c r="G146" s="2"/>
-    </row>
-    <row r="147" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+      <c r="F146" s="2"/>
+    </row>
+    <row r="147" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A147" s="4" t="s">
         <v>35</v>
       </c>
@@ -3814,12 +3439,9 @@
       <c r="E147" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="F147" s="4">
-        <v>3</v>
-      </c>
-      <c r="G147" s="4"/>
-    </row>
-    <row r="148" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+      <c r="F147" s="4"/>
+    </row>
+    <row r="148" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A148" s="4" t="s">
         <v>24</v>
       </c>
@@ -3835,14 +3457,11 @@
       <c r="E148" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="F148" s="4">
-        <v>1</v>
-      </c>
-      <c r="G148" s="2">
+      <c r="F148" s="2">
         <v>3</v>
       </c>
     </row>
-    <row r="149" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A149" s="4" t="s">
         <v>24</v>
       </c>
@@ -3861,11 +3480,8 @@
       <c r="F149" s="4">
         <v>3</v>
       </c>
-      <c r="G149" s="4">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="150" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+    </row>
+    <row r="150" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A150" s="4" t="s">
         <v>74</v>
       </c>
@@ -3881,12 +3497,9 @@
       <c r="E150" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="F150" s="4">
-        <v>3</v>
-      </c>
-      <c r="G150" s="4"/>
-    </row>
-    <row r="151" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+      <c r="F150" s="4"/>
+    </row>
+    <row r="151" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A151" s="4" t="s">
         <v>36</v>
       </c>
@@ -3902,12 +3515,9 @@
       <c r="E151" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="F151" s="4">
-        <v>1</v>
-      </c>
-      <c r="G151" s="2"/>
-    </row>
-    <row r="152" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+      <c r="F151" s="2"/>
+    </row>
+    <row r="152" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A152" s="4" t="s">
         <v>36</v>
       </c>
@@ -3923,12 +3533,9 @@
       <c r="E152" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="F152" s="4">
-        <v>3</v>
-      </c>
-      <c r="G152" s="4"/>
-    </row>
-    <row r="153" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+      <c r="F152" s="4"/>
+    </row>
+    <row r="153" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A153" s="4" t="s">
         <v>17</v>
       </c>
@@ -3944,14 +3551,11 @@
       <c r="E153" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="F153" s="4">
-        <v>0</v>
-      </c>
-      <c r="G153" s="2">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="154" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+      <c r="F153" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="154" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A154" s="4" t="s">
         <v>17</v>
       </c>
@@ -3967,16 +3571,13 @@
       <c r="E154" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="F154" s="4">
-        <v>2</v>
-      </c>
-      <c r="G154" s="2">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="155" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F154" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="155" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A155" s="4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B155" s="4">
         <v>97690</v>
@@ -3988,14 +3589,11 @@
         <v>12</v>
       </c>
       <c r="E155" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="F155" s="4">
-        <v>5</v>
-      </c>
-      <c r="G155" s="4"/>
-    </row>
-    <row r="156" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>100</v>
+      </c>
+      <c r="F155" s="4"/>
+    </row>
+    <row r="156" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A156" s="4" t="s">
         <v>21</v>
       </c>
@@ -4011,12 +3609,9 @@
       <c r="E156" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="F156" s="4">
-        <v>4</v>
-      </c>
-      <c r="G156" s="4"/>
-    </row>
-    <row r="157" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F156" s="4"/>
+    </row>
+    <row r="157" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A157" s="4" t="s">
         <v>21</v>
       </c>
@@ -4032,12 +3627,9 @@
       <c r="E157" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="F157" s="4">
-        <v>1</v>
-      </c>
-      <c r="G157" s="2"/>
-    </row>
-    <row r="158" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F157" s="2"/>
+    </row>
+    <row r="158" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A158" s="4" t="s">
         <v>21</v>
       </c>
@@ -4053,12 +3645,9 @@
       <c r="E158" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="F158" s="4">
-        <v>3</v>
-      </c>
-      <c r="G158" s="4"/>
-    </row>
-    <row r="159" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F158" s="4"/>
+    </row>
+    <row r="159" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A159" s="4" t="s">
         <v>88</v>
       </c>
@@ -4074,12 +3663,9 @@
       <c r="E159" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="F159" s="4">
-        <v>3</v>
-      </c>
-      <c r="G159" s="4"/>
-    </row>
-    <row r="160" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F159" s="4"/>
+    </row>
+    <row r="160" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A160" s="4" t="s">
         <v>71</v>
       </c>
@@ -4095,12 +3681,9 @@
       <c r="E160" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="F160" s="4">
-        <v>3</v>
-      </c>
-      <c r="G160" s="4"/>
-    </row>
-    <row r="161" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F160" s="4"/>
+    </row>
+    <row r="161" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A161" s="4" t="s">
         <v>81</v>
       </c>
@@ -4119,10 +3702,9 @@
       <c r="F161" s="4">
         <v>3</v>
       </c>
-      <c r="G161" s="4"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G161">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F161">
     <sortCondition ref="B2:B161"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>